<commit_message>
update skill report - add inconsistent data
</commit_message>
<xml_diff>
--- a/table-export-004.xlsx
+++ b/table-export-004.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raksmey\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aupp-my.sharepoint.com/personal/s_chea_aupp_edu_kh1/Documents/AUPP Class/INF652/class_resources/chapter_01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BE3BD811-F8C7-40D3-99D2-13F5FB7B3026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:40009_{BE3BD811-F8C7-40D3-99D2-13F5FB7B3026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AD59DFF-ACDF-4EF2-A396-B5BF654323C3}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table-export-004" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Skill3Date</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
     <t>Programming</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>Communication</t>
   </si>
   <si>
-    <t>Programmer</t>
-  </si>
-  <si>
     <t>Microsoft</t>
   </si>
   <si>
@@ -101,12 +95,31 @@
   </si>
   <si>
     <t>Technician</t>
+  </si>
+  <si>
+    <t>Programing</t>
+  </si>
+  <si>
+    <t>Excell</t>
+  </si>
+  <si>
+    <t>John12</t>
+  </si>
+  <si>
+    <t>Programmers</t>
+  </si>
+  <si>
+    <t>Communication_101</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,10 +612,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -957,11 +972,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -971,7 +986,7 @@
     <col min="4" max="4" width="18.26953125" customWidth="1"/>
     <col min="5" max="5" width="10.36328125" customWidth="1"/>
     <col min="6" max="6" width="16.26953125" customWidth="1"/>
-    <col min="7" max="7" width="14.1796875" customWidth="1"/>
+    <col min="7" max="7" width="23.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.90625" customWidth="1"/>
     <col min="9" max="9" width="16.08984375" customWidth="1"/>
     <col min="10" max="10" width="18.1796875" customWidth="1"/>
@@ -1021,26 +1036,26 @@
         <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="2">
         <v>43966</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2">
         <v>43966</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2">
+        <v>13</v>
+      </c>
+      <c r="K2" s="3">
         <v>44027</v>
       </c>
     </row>
@@ -1053,19 +1068,19 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -1077,10 +1092,10 @@
         <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2">
         <v>43777</v>
@@ -1090,13 +1105,13 @@
         <v>44280</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4" s="2">
         <v>44145</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -1129,14 +1144,14 @@
         <v>105</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="2">
         <v>44387</v>
@@ -1144,7 +1159,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="K6" s="2">
         <v>44413</v>
@@ -1159,13 +1174,13 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
         <v>44956</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="G7" s="2">
         <v>44972</v>
@@ -1183,7 +1198,7 @@
         <v>107</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="2">
@@ -1192,7 +1207,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1208,20 +1223,20 @@
         <v>108</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="2">
+        <v>13</v>
+      </c>
+      <c r="G9" s="4">
         <v>43992</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="2">
         <v>44013</v>
@@ -1242,13 +1257,13 @@
         <v>44535</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10" s="1"/>
     </row>
@@ -1261,19 +1276,19 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I11" s="2">
         <v>45056</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K11" s="1"/>
     </row>

</xml_diff>